<commit_message>
fixed Template and separate Skyridge and SBL
</commit_message>
<xml_diff>
--- a/reporting/report_template/SkyRidge_CLO_ABS_Template.xlsx
+++ b/reporting/report_template/SkyRidge_CLO_ABS_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XiaHanlu\workspace\legacyReporting\reporting\report_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF6E671-8E8C-47C7-9C29-DBD2E4E3AE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC8DC09-36FB-4BAD-8284-14490481A117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Disclaimer" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -5697,28 +5697,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -5800,28 +5778,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -5878,86 +5834,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-      </font>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-      </font>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -7146,6 +7022,28 @@
         <name val="Arial"/>
         <family val="2"/>
       </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+      </font>
       <alignment horizontal="center" vertical="bottom"/>
     </dxf>
     <dxf>
@@ -7194,6 +7092,28 @@
         <name val="Arial"/>
         <family val="2"/>
       </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+      </font>
       <alignment horizontal="center" vertical="bottom"/>
     </dxf>
     <dxf>
@@ -7227,6 +7147,28 @@
         <name val="Arial"/>
         <family val="2"/>
       </font>
+      <alignment horizontal="center" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom"/>
     </dxf>
     <dxf>
@@ -9761,6 +9703,18 @@
     <dxf>
       <font>
         <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
@@ -9771,6 +9725,30 @@
         <name val="Arial"/>
         <family val="2"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </dxf>
     <dxf>
       <font>
@@ -9844,6 +9822,17 @@
     <dxf>
       <font>
         <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+      </font>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
@@ -9855,6 +9844,17 @@
         <family val="2"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+      </font>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -10221,35 +10221,35 @@
   <autoFilter ref="B38:I47" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Manager Name" totalsRowLabel="Total" dataDxfId="281" totalsRowDxfId="280"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Current Face" dataDxfId="19" totalsRowDxfId="279" dataCellStyle="Comma">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Current Face" dataDxfId="279" totalsRowDxfId="278" dataCellStyle="Comma">
       <calculatedColumnFormula>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Market Value" dataDxfId="18" totalsRowDxfId="278" dataCellStyle="Comma">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Market Value" dataDxfId="277" totalsRowDxfId="276" dataCellStyle="Comma">
       <calculatedColumnFormula>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Current Face %" dataDxfId="277" totalsRowDxfId="276" dataCellStyle="Percent">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Current Face %" dataDxfId="275" totalsRowDxfId="274" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$37,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Market Value %" dataDxfId="275" totalsRowDxfId="274" dataCellStyle="Percent">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Market Value %" dataDxfId="273" totalsRowDxfId="272" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$37,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. of Issuers" dataDxfId="17">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. of Issuers" dataDxfId="271">
       <calculatedColumnFormula array="1">IF($C$4="All Portfolios",
    COUNTA(_xlfn.UNIQUE(_xlfn._xlws.FILTER(tbl_rawhold[Issuer Name],tbl_rawhold[Manager]= tbl_report_manager[[#This Row],[Manager Name]]))),
     COUNTA(_xlfn.UNIQUE(_xlfn._xlws.FILTER(tbl_rawhold[Issuer Name], (tbl_rawhold[Manager]= tbl_report_manager[[#This Row],[Manager Name]])*(tbl_rawhold[Portfolio_Name]= $C$4))))
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="No. of Cusips" dataDxfId="16" totalsRowDxfId="273">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="No. of Cusips" dataDxfId="270" totalsRowDxfId="269">
       <calculatedColumnFormula array="1">IF($C$4="All Portfolios",
    COUNTA(_xlfn.UNIQUE(_xlfn._xlws.FILTER(tbl_rawhold[CUSIP],tbl_rawhold[Manager]= tbl_report_manager[[#This Row],[Manager Name]]))),
     COUNTA(_xlfn.UNIQUE(_xlfn._xlws.FILTER(tbl_rawhold[CUSIP], (tbl_rawhold[Manager]= tbl_report_manager[[#This Row],[Manager Name]])*(tbl_rawhold[Portfolio_Name]= $C$4))))
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="No. of Positions" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="272">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="No. of Positions" totalsRowFunction="sum" dataDxfId="268" totalsRowDxfId="267">
       <calculatedColumnFormula>IF($C$4="All Portfolios",
    COUNTIFS(tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    COUNTIFS(tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]])
@@ -10261,57 +10261,57 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="tbl_hold_b" displayName="tbl_hold_b" ref="B118:S121" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="tbl_hold_b" displayName="tbl_hold_b" ref="B118:S121" totalsRowShown="0" headerRowDxfId="118" dataDxfId="117">
   <autoFilter ref="B118:S121" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Cusip" dataDxfId="121"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Issuer" dataDxfId="120"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Security Description" dataDxfId="119"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="Issue Date" dataDxfId="118"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Maturity Date" dataDxfId="117"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="Coupon" dataDxfId="116"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="Spread" dataDxfId="115"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0900-000008000000}" name="Current Face" dataDxfId="114" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0900-000009000000}" name="Factor" dataDxfId="113"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0900-00000A000000}" name="Market Price" dataDxfId="112"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0900-00000B000000}" name="Market Value" dataDxfId="111" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0900-00000C000000}" name="NRSRO" dataDxfId="110"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0900-00000D000000}" name="NRSRO Rating" dataDxfId="109"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0900-00000E000000}" name="WAL" dataDxfId="108"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0900-00000F000000}" name="Par Sub" dataDxfId="107" dataCellStyle="Percent"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0900-000010000000}" name="Implied DM" dataDxfId="106"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0900-000011000000}" name="Next Payment Date" dataDxfId="105"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0900-000012000000}" name="Non-Call Date" dataDxfId="104"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Cusip" dataDxfId="116"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Issuer" dataDxfId="115"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Security Description" dataDxfId="114"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="Issue Date" dataDxfId="113"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Maturity Date" dataDxfId="112"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="Coupon" dataDxfId="111"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="Spread" dataDxfId="110"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0900-000008000000}" name="Current Face" dataDxfId="109" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0900-000009000000}" name="Factor" dataDxfId="108"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0900-00000A000000}" name="Market Price" dataDxfId="107"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0900-00000B000000}" name="Market Value" dataDxfId="106" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0900-00000C000000}" name="NRSRO" dataDxfId="105"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0900-00000D000000}" name="NRSRO Rating" dataDxfId="104"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0900-00000E000000}" name="WAL" dataDxfId="103"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0900-00000F000000}" name="Par Sub" dataDxfId="102" dataCellStyle="Percent"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0900-000010000000}" name="Implied DM" dataDxfId="101"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0900-000011000000}" name="Next Payment Date" dataDxfId="100"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0900-000012000000}" name="Non-Call Date" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Table11" displayName="Table11" ref="B9:C18" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Table11" displayName="Table11" ref="B9:C18" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
   <autoFilter ref="B9:C18" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Analytics" dataDxfId="101"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="CLO/ABS Debt" dataDxfId="100"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Analytics" dataDxfId="96"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="CLO/ABS Debt" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table13" displayName="Table13" ref="E9:G18" totalsRowCount="1" headerRowDxfId="99" dataDxfId="98" totalsRowDxfId="97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table13" displayName="Table13" ref="E9:G18" totalsRowCount="1" headerRowDxfId="94" dataDxfId="93" totalsRowDxfId="92">
   <autoFilter ref="E9:G17" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Tranche Rating" totalsRowLabel="Total" dataDxfId="96" totalsRowDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Portfolio % CF" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="12" dataCellStyle="Percent">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Tranche Rating" totalsRowLabel="Total" dataDxfId="91" totalsRowDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Portfolio % CF" totalsRowFunction="sum" dataDxfId="90" totalsRowDxfId="10" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="Portfolio % MV" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="11" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="Portfolio % MV" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="9" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</calculatedColumnFormula>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -10319,19 +10319,19 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table14" displayName="Table14" ref="I9:K17" totalsRowCount="1" headerRowDxfId="95" dataDxfId="94" totalsRowDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table14" displayName="Table14" ref="I9:K17" totalsRowCount="1" headerRowDxfId="89" dataDxfId="88" totalsRowDxfId="87">
   <autoFilter ref="I9:K16" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="WAL" totalsRowLabel="Total" dataDxfId="92" totalsRowDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Portfolio % CF" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="7" dataCellStyle="Percent">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="WAL" totalsRowLabel="Total" dataDxfId="86" totalsRowDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Portfolio % CF" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="6" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]])/$C$10,
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Portfolio % MV" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="6" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Portfolio % MV" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="5" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</calculatedColumnFormula>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -10339,19 +10339,19 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table15" displayName="Table15" ref="M9:O16" totalsRowCount="1" headerRowDxfId="91" dataDxfId="90" totalsRowDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table15" displayName="Table15" ref="M9:O16" totalsRowCount="1" headerRowDxfId="84" dataDxfId="83" totalsRowDxfId="82">
   <autoFilter ref="M9:O15" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Coupon" totalsRowLabel="Total" dataDxfId="88" totalsRowDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Portfolio % CF" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="2" dataCellStyle="Percent">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Coupon" totalsRowLabel="Total" dataDxfId="81" totalsRowDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Portfolio % CF" totalsRowFunction="sum" dataDxfId="80" totalsRowDxfId="2" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]])/$C$10,
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="Portfolio % MV" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</calculatedColumnFormula>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -10359,68 +10359,68 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="tbl_hold_ccc" displayName="tbl_hold_ccc" ref="B128:S129" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="tbl_hold_ccc" displayName="tbl_hold_ccc" ref="B128:S129" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
   <autoFilter ref="B128:S129" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="Cusip" dataDxfId="85"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="Issuer" dataDxfId="84"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="Security Description" dataDxfId="83"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="Issue Date" dataDxfId="82"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0E00-000005000000}" name="Maturity Date" dataDxfId="81"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0E00-000006000000}" name="Coupon" dataDxfId="80"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0E00-000007000000}" name="Spread" dataDxfId="79"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0E00-000008000000}" name="Current Face" dataDxfId="78" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0E00-000009000000}" name="Factor" dataDxfId="77"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0E00-00000A000000}" name="Market Price" dataDxfId="76"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0E00-00000B000000}" name="Market Value" dataDxfId="75" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0E00-00000C000000}" name="NRSRO" dataDxfId="74"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0E00-00000D000000}" name="NRSRO Rating" dataDxfId="73"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0E00-00000E000000}" name="WAL" dataDxfId="72"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0E00-00000F000000}" name="Par Sub" dataDxfId="71" dataCellStyle="Percent"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0E00-000010000000}" name="Implied DM" dataDxfId="70"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0E00-000011000000}" name="Next Payment Date" dataDxfId="69"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0E00-000012000000}" name="Non-Call Date" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="Cusip" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="Issuer" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="Security Description" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="Issue Date" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0E00-000005000000}" name="Maturity Date" dataDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0E00-000006000000}" name="Coupon" dataDxfId="72"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0E00-000007000000}" name="Spread" dataDxfId="71"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0E00-000008000000}" name="Current Face" dataDxfId="70" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0E00-000009000000}" name="Factor" dataDxfId="69"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0E00-00000A000000}" name="Market Price" dataDxfId="68"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0E00-00000B000000}" name="Market Value" dataDxfId="67" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0E00-00000C000000}" name="NRSRO" dataDxfId="66"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0E00-00000D000000}" name="NRSRO Rating" dataDxfId="65"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0E00-00000E000000}" name="WAL" dataDxfId="64"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0E00-00000F000000}" name="Par Sub" dataDxfId="63" dataCellStyle="Percent"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0E00-000010000000}" name="Implied DM" dataDxfId="62"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0E00-000011000000}" name="Next Payment Date" dataDxfId="61"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0E00-000012000000}" name="Non-Call Date" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="tbl_hold_nr" displayName="tbl_hold_nr" ref="B136:S137" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="tbl_hold_nr" displayName="tbl_hold_nr" ref="B136:S137" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="B136:S137" xr:uid="{00000000-0009-0000-0100-000010000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="Cusip" dataDxfId="65"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="Issuer" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="Security Description" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="Issue Date" dataDxfId="62"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0F00-000005000000}" name="Maturity Date" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0F00-000006000000}" name="Coupon" dataDxfId="60"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0F00-000007000000}" name="Spread" dataDxfId="59"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0F00-000008000000}" name="Current Face" dataDxfId="58" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0F00-000009000000}" name="Factor" dataDxfId="57"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0F00-00000A000000}" name="Market Price" dataDxfId="56"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0F00-00000B000000}" name="Market Value" dataDxfId="55" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0F00-00000C000000}" name="NRSRO" dataDxfId="54"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0F00-00000D000000}" name="NRSRO Rating" dataDxfId="53"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0F00-00000E000000}" name="WAL" dataDxfId="52"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0F00-00000F000000}" name="Par Sub" dataDxfId="51" dataCellStyle="Percent"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0F00-000010000000}" name="Implied DM" dataDxfId="50"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0F00-000011000000}" name="Next Payment Date" dataDxfId="49"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0F00-000012000000}" name="Non-Call Date" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="Cusip" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="Issuer" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="Security Description" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="Issue Date" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0F00-000005000000}" name="Maturity Date" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0F00-000006000000}" name="Coupon" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0F00-000007000000}" name="Spread" dataDxfId="51"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0F00-000008000000}" name="Current Face" dataDxfId="50" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0F00-000009000000}" name="Factor" dataDxfId="49"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0F00-00000A000000}" name="Market Price" dataDxfId="48"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0F00-00000B000000}" name="Market Value" dataDxfId="47" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0F00-00000C000000}" name="NRSRO" dataDxfId="46"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0F00-00000D000000}" name="NRSRO Rating" dataDxfId="45"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0F00-00000E000000}" name="WAL" dataDxfId="44"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0F00-00000F000000}" name="Par Sub" dataDxfId="43" dataCellStyle="Percent"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0F00-000010000000}" name="Implied DM" dataDxfId="42"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0F00-000011000000}" name="Next Payment Date" dataDxfId="41"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0F00-000012000000}" name="Non-Call Date" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="tbl_rawtran" displayName="tbl_rawtran" ref="A1:L130" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="tbl_rawtran" displayName="tbl_rawtran" ref="A1:L130" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37">
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="Portfolio"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="Security ID"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-1000-000004000000}" name="Security Description"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="Trade Date" dataDxfId="44"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" name="Settle Date" dataDxfId="43"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1000-000007000000}" name="Maturity Date" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="Trade Date" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" name="Settle Date" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1000-000007000000}" name="Maturity Date" dataDxfId="34"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-1000-000008000000}" name="Quantity"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-1000-000009000000}" name="Price"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-1000-00000A000000}" name="Cost Proceeds"/>
@@ -10433,214 +10433,214 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{908C9144-5168-489A-B4C5-8E14FBC64E8B}" name="tbl_rawhold" displayName="tbl_rawhold" ref="A1:S644" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{908C9144-5168-489A-B4C5-8E14FBC64E8B}" name="tbl_rawhold" displayName="tbl_rawhold" ref="A1:S644" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" tableBorderDxfId="31">
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{55FCBEB5-6900-4A67-BD6C-5A9D896E1F5B}" name="Portfolio Code" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{B1CF8769-6374-435A-B341-04B6530C6DC0}" name="Investment Type" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{A07ABB32-648E-4DC0-8A63-C5E80A371954}" name="CUSIP" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{556E6DBB-32B8-496E-8193-535B4BC44D5E}" name="Current Face" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{C5524FEB-E9AD-41AF-A7A9-675F9F7B6BB8}" name="BASEMarket Value" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{C29BC4EB-05CE-4504-AC69-A931E39C1175}" name="BASEOriginal Cost" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{3E560A71-647E-40B5-B1F1-22ADC8BA51E3}" name="Issuer Name" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{8126FEFE-EFEC-4135-9477-8694863B6BA7}" name="Coupon Rate" dataDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{8FB7B91A-A940-4697-B398-26602BF5D2F2}" name="Security Description" dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{D8168212-3492-42EF-B3A8-C72605D51A83}" name="Maturity Date" dataDxfId="29"/>
-    <tableColumn id="11" xr3:uid="{4761EF4A-49D2-426F-81D7-A446683B41F2}" name="Spread" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{40DED1B9-3704-443E-B599-31BA55E5CB3A}" name="Factor" dataDxfId="27"/>
-    <tableColumn id="13" xr3:uid="{A5DBBD08-04CF-4978-8742-ACBE8366B0E3}" name="Portfolio_Name" dataDxfId="26"/>
-    <tableColumn id="14" xr3:uid="{05CD9835-194F-4CF2-9481-2CE94E520220}" name="Row Labels" dataDxfId="25"/>
-    <tableColumn id="15" xr3:uid="{4FDD0F14-7987-4EEE-9956-BC970244E1B9}" name="Manager" dataDxfId="24"/>
-    <tableColumn id="16" xr3:uid="{F362AD71-77A1-4E4C-8546-33675A4AEB36}" name="WAL" dataDxfId="23"/>
-    <tableColumn id="17" xr3:uid="{8E7029B9-8AA8-401F-B6EA-6007BA7FC880}" name="Tranche Rating" dataDxfId="22"/>
-    <tableColumn id="18" xr3:uid="{065572E1-697D-4400-99B2-60F27DAFB9E4}" name="WAL_Range" dataDxfId="21"/>
-    <tableColumn id="19" xr3:uid="{6B3E49EE-3D56-4DE1-A9CB-C256FD63AB95}" name="coupon_Range" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{55FCBEB5-6900-4A67-BD6C-5A9D896E1F5B}" name="Portfolio Code" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{B1CF8769-6374-435A-B341-04B6530C6DC0}" name="Investment Type" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{A07ABB32-648E-4DC0-8A63-C5E80A371954}" name="CUSIP" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{556E6DBB-32B8-496E-8193-535B4BC44D5E}" name="Current Face" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{C5524FEB-E9AD-41AF-A7A9-675F9F7B6BB8}" name="BASEMarket Value" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{C29BC4EB-05CE-4504-AC69-A931E39C1175}" name="BASEOriginal Cost" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{3E560A71-647E-40B5-B1F1-22ADC8BA51E3}" name="Issuer Name" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{8126FEFE-EFEC-4135-9477-8694863B6BA7}" name="Coupon Rate" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{8FB7B91A-A940-4697-B398-26602BF5D2F2}" name="Security Description" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{D8168212-3492-42EF-B3A8-C72605D51A83}" name="Maturity Date" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{4761EF4A-49D2-426F-81D7-A446683B41F2}" name="Spread" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{40DED1B9-3704-443E-B599-31BA55E5CB3A}" name="Factor" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{A5DBBD08-04CF-4978-8742-ACBE8366B0E3}" name="Portfolio_Name" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{05CD9835-194F-4CF2-9481-2CE94E520220}" name="Row Labels" dataDxfId="17"/>
+    <tableColumn id="15" xr3:uid="{4FDD0F14-7987-4EEE-9956-BC970244E1B9}" name="Manager" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{F362AD71-77A1-4E4C-8546-33675A4AEB36}" name="WAL" dataDxfId="15"/>
+    <tableColumn id="17" xr3:uid="{8E7029B9-8AA8-401F-B6EA-6007BA7FC880}" name="Tranche Rating" dataDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{065572E1-697D-4400-99B2-60F27DAFB9E4}" name="WAL_Range" dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{6B3E49EE-3D56-4DE1-A9CB-C256FD63AB95}" name="coupon_Range" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tbl_report_paydown" displayName="tbl_report_paydown" ref="B52:H53" totalsRowShown="0" headerRowDxfId="271" dataDxfId="270">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tbl_report_paydown" displayName="tbl_report_paydown" ref="B52:H53" totalsRowShown="0" headerRowDxfId="266" dataDxfId="265">
   <autoFilter ref="B52:H53" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Type" dataDxfId="269"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Issuer" dataDxfId="268"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Security Description" dataDxfId="267"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Cusip" dataDxfId="266"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Settle Date" dataDxfId="265"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Face Value" dataDxfId="264" dataCellStyle="Comma"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Tranche Rating" dataDxfId="263"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Type" dataDxfId="264"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Issuer" dataDxfId="263"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Security Description" dataDxfId="262"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Cusip" dataDxfId="261"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Settle Date" dataDxfId="260"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Face Value" dataDxfId="259" dataCellStyle="Comma"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Tranche Rating" dataDxfId="258"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tbl_report_sale" displayName="tbl_report_sale" ref="B59:J60" totalsRowShown="0" headerRowDxfId="262">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tbl_report_sale" displayName="tbl_report_sale" ref="B59:J60" totalsRowShown="0" headerRowDxfId="257">
   <autoFilter ref="B59:J60" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Issuer" dataDxfId="261"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Security Description" dataDxfId="260"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Cusip" dataDxfId="259"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Trade Date" dataDxfId="258"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Settle Date" dataDxfId="257"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Face Value" dataDxfId="256" dataCellStyle="Comma"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Sale Price" dataDxfId="255"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Maturity Date" dataDxfId="254"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Tranche Rating" dataDxfId="253"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Issuer" dataDxfId="256"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Security Description" dataDxfId="255"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Cusip" dataDxfId="254"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Trade Date" dataDxfId="253"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Settle Date" dataDxfId="252"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Face Value" dataDxfId="251" dataCellStyle="Comma"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Sale Price" dataDxfId="250"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Maturity Date" dataDxfId="249"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Tranche Rating" dataDxfId="248"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="tbl_report_purchase" displayName="tbl_report_purchase" ref="B67:J68" totalsRowShown="0" headerRowDxfId="252">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="tbl_report_purchase" displayName="tbl_report_purchase" ref="B67:J68" totalsRowShown="0" headerRowDxfId="247">
   <autoFilter ref="B67:J68" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Issuer" dataDxfId="251"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Security Description" dataDxfId="250"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Cusip" dataDxfId="249"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Trade Date" dataDxfId="248"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Settle Date" dataDxfId="247"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Face Value" dataDxfId="246" dataCellStyle="Comma"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Purchase Price" dataDxfId="245"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Maturity Date" dataDxfId="244"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Tranche Rating" dataDxfId="243"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Issuer" dataDxfId="246"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Security Description" dataDxfId="245"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Cusip" dataDxfId="244"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Trade Date" dataDxfId="243"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Settle Date" dataDxfId="242"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Face Value" dataDxfId="241" dataCellStyle="Comma"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Purchase Price" dataDxfId="240"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Maturity Date" dataDxfId="239"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Tranche Rating" dataDxfId="238"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="tbl_hold_aaa" displayName="tbl_hold_aaa" ref="B75:S76" totalsRowShown="0" headerRowDxfId="242" dataDxfId="241">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="tbl_hold_aaa" displayName="tbl_hold_aaa" ref="B75:S76" totalsRowShown="0" headerRowDxfId="237" dataDxfId="236">
   <autoFilter ref="B75:S76" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Cusip" dataDxfId="240"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Issuer" dataDxfId="239"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Security Description" dataDxfId="238"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Issue Date" dataDxfId="237"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Maturity Date" dataDxfId="236"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Coupon" dataDxfId="235"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Spread" dataDxfId="234"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Current Face" dataDxfId="233" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Factor" dataDxfId="232"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="Market Price" dataDxfId="231"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="Market Value" dataDxfId="230" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="NRSRO" dataDxfId="229"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0400-00000D000000}" name="NRSRO Rating" dataDxfId="228"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0400-00000E000000}" name="WAL" dataDxfId="227"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0400-00000F000000}" name="Par Sub" dataDxfId="226" dataCellStyle="Percent"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0400-000010000000}" name="Implied DM" dataDxfId="225"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0400-000011000000}" name="Next Payment Date" dataDxfId="224"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0400-000012000000}" name="Non-Call Date" dataDxfId="223"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Cusip" dataDxfId="235"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Issuer" dataDxfId="234"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Security Description" dataDxfId="233"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Issue Date" dataDxfId="232"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Maturity Date" dataDxfId="231"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Coupon" dataDxfId="230"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Spread" dataDxfId="229"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Current Face" dataDxfId="228" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Factor" dataDxfId="227"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="Market Price" dataDxfId="226"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="Market Value" dataDxfId="225" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="NRSRO" dataDxfId="224"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0400-00000D000000}" name="NRSRO Rating" dataDxfId="223"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0400-00000E000000}" name="WAL" dataDxfId="222"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0400-00000F000000}" name="Par Sub" dataDxfId="221" dataCellStyle="Percent"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0400-000010000000}" name="Implied DM" dataDxfId="220"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0400-000011000000}" name="Next Payment Date" dataDxfId="219"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0400-000012000000}" name="Non-Call Date" dataDxfId="218"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="tbl_hold_aa" displayName="tbl_hold_aa" ref="B83:S86" totalsRowShown="0" headerRowDxfId="222" dataDxfId="221">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="tbl_hold_aa" displayName="tbl_hold_aa" ref="B83:S86" totalsRowShown="0" headerRowDxfId="217" dataDxfId="216">
   <autoFilter ref="B83:S86" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Cusip" dataDxfId="220"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Issuer" dataDxfId="219"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Security Description" dataDxfId="218"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Issue Date" dataDxfId="217"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Maturity Date" dataDxfId="216"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Coupon" dataDxfId="215"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Spread" dataDxfId="214"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Current Face" dataDxfId="213"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="Factor" dataDxfId="212"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="Market Price" dataDxfId="211"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="Market Value" dataDxfId="210"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NRSRO" dataDxfId="209"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="NRSRO Rating" dataDxfId="208"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0500-00000E000000}" name="WAL" dataDxfId="207"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Par Sub" dataDxfId="206"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Implied DM" dataDxfId="205"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Next Payment Date" dataDxfId="204"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0500-000012000000}" name="Non-Call Date" dataDxfId="203"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Cusip" dataDxfId="215"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Issuer" dataDxfId="214"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Security Description" dataDxfId="213"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Issue Date" dataDxfId="212"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Maturity Date" dataDxfId="211"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Coupon" dataDxfId="210"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Spread" dataDxfId="209"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Current Face" dataDxfId="208"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="Factor" dataDxfId="207"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="Market Price" dataDxfId="206"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="Market Value" dataDxfId="205"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NRSRO" dataDxfId="204"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="NRSRO Rating" dataDxfId="203"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0500-00000E000000}" name="WAL" dataDxfId="202"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Par Sub" dataDxfId="201"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Implied DM" dataDxfId="200"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Next Payment Date" dataDxfId="199"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0500-000012000000}" name="Non-Call Date" dataDxfId="198"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="tbl_hold_a" displayName="tbl_hold_a" ref="B93:S95" headerRowDxfId="202" dataDxfId="201" totalsRowDxfId="200">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="tbl_hold_a" displayName="tbl_hold_a" ref="B93:S95" headerRowDxfId="197" dataDxfId="196" totalsRowDxfId="195">
   <autoFilter ref="B93:S95" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Cusip" totalsRowLabel="Total" dataDxfId="199" totalsRowDxfId="198"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Issuer" dataDxfId="197" totalsRowDxfId="196"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Security Description" dataDxfId="195" totalsRowDxfId="194"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Issue Date" dataDxfId="193" totalsRowDxfId="192"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Maturity Date" dataDxfId="191" totalsRowDxfId="190"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Coupon" dataDxfId="189" totalsRowDxfId="188"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Spread" dataDxfId="187" totalsRowDxfId="186"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Current Face" dataDxfId="185" totalsRowDxfId="184" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Factor" dataDxfId="183" totalsRowDxfId="182"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Market Price" dataDxfId="181" totalsRowDxfId="180"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Market Value" dataDxfId="179" totalsRowDxfId="178" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="NRSRO" dataDxfId="177" totalsRowDxfId="176"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="NRSRO Rating" dataDxfId="175" totalsRowDxfId="174"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="WAL" dataDxfId="173" totalsRowDxfId="172"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Par Sub" dataDxfId="171" totalsRowDxfId="170" dataCellStyle="Percent"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Implied DM" dataDxfId="169" totalsRowDxfId="168"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0600-000011000000}" name="Next Payment Date" dataDxfId="167" totalsRowDxfId="166"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0600-000012000000}" name="Non-Call Date" totalsRowFunction="sum" dataDxfId="165" totalsRowDxfId="164"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Cusip" totalsRowLabel="Total" dataDxfId="194" totalsRowDxfId="193"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Issuer" dataDxfId="192" totalsRowDxfId="191"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Security Description" dataDxfId="190" totalsRowDxfId="189"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Issue Date" dataDxfId="188" totalsRowDxfId="187"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Maturity Date" dataDxfId="186" totalsRowDxfId="185"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Coupon" dataDxfId="184" totalsRowDxfId="183"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Spread" dataDxfId="182" totalsRowDxfId="181"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Current Face" dataDxfId="180" totalsRowDxfId="179" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Factor" dataDxfId="178" totalsRowDxfId="177"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Market Price" dataDxfId="176" totalsRowDxfId="175"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Market Value" dataDxfId="174" totalsRowDxfId="173" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="NRSRO" dataDxfId="172" totalsRowDxfId="171"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="NRSRO Rating" dataDxfId="170" totalsRowDxfId="169"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="WAL" dataDxfId="168" totalsRowDxfId="167"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Par Sub" dataDxfId="166" totalsRowDxfId="165" dataCellStyle="Percent"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Implied DM" dataDxfId="164" totalsRowDxfId="163"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0600-000011000000}" name="Next Payment Date" dataDxfId="162" totalsRowDxfId="161"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0600-000012000000}" name="Non-Call Date" totalsRowFunction="sum" dataDxfId="160" totalsRowDxfId="159"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="tbl_hold_bbb" displayName="tbl_hold_bbb" ref="B102:S103" totalsRowShown="0" headerRowDxfId="163" dataDxfId="162">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="tbl_hold_bbb" displayName="tbl_hold_bbb" ref="B102:S103" totalsRowShown="0" headerRowDxfId="158" dataDxfId="157">
   <autoFilter ref="B102:S103" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Cusip" dataDxfId="161"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Issuer" dataDxfId="160"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Security Description" dataDxfId="159"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Issue Date" dataDxfId="158"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Maturity Date" dataDxfId="157"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Coupon" dataDxfId="156"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Spread" dataDxfId="155"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Current Face" dataDxfId="154" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Factor" dataDxfId="153"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Market Price" dataDxfId="152"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Market Value" dataDxfId="151" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="NRSRO" dataDxfId="150"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="NRSRO Rating" dataDxfId="149"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0700-00000E000000}" name="WAL" dataDxfId="148"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0700-00000F000000}" name="Par Sub" dataDxfId="147" dataCellStyle="Percent"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0700-000010000000}" name="Implied DM" dataDxfId="146"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0700-000011000000}" name="Next Payment Date" dataDxfId="145"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0700-000012000000}" name="Non-Call Date" dataDxfId="144"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Cusip" dataDxfId="156"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Issuer" dataDxfId="155"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Security Description" dataDxfId="154"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Issue Date" dataDxfId="153"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Maturity Date" dataDxfId="152"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Coupon" dataDxfId="151"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Spread" dataDxfId="150"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Current Face" dataDxfId="149" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Factor" dataDxfId="148"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Market Price" dataDxfId="147"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Market Value" dataDxfId="146" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="NRSRO" dataDxfId="145"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="NRSRO Rating" dataDxfId="144"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0700-00000E000000}" name="WAL" dataDxfId="143"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0700-00000F000000}" name="Par Sub" dataDxfId="142" dataCellStyle="Percent"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0700-000010000000}" name="Implied DM" dataDxfId="141"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0700-000011000000}" name="Next Payment Date" dataDxfId="140"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0700-000012000000}" name="Non-Call Date" dataDxfId="139"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="tbl_hold_bb" displayName="tbl_hold_bb" ref="B110:S111" totalsRowShown="0" headerRowDxfId="143" dataDxfId="142">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="tbl_hold_bb" displayName="tbl_hold_bb" ref="B110:S111" totalsRowShown="0" headerRowDxfId="138" dataDxfId="137">
   <autoFilter ref="B110:S111" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Cusip" dataDxfId="141"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Issuer" dataDxfId="140"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Security Description" dataDxfId="139"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Issue Date" dataDxfId="138"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Maturity Date" dataDxfId="137"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Coupon" dataDxfId="136"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="Spread" dataDxfId="135"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="Current Face" dataDxfId="134" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="Factor" dataDxfId="133"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="Market Price" dataDxfId="132"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="Market Value" dataDxfId="131" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="NRSRO" dataDxfId="130"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0800-00000D000000}" name="NRSRO Rating" dataDxfId="129"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0800-00000E000000}" name="WAL" dataDxfId="128"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0800-00000F000000}" name="Par Sub" dataDxfId="127" dataCellStyle="Percent"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0800-000010000000}" name="Implied DM" dataDxfId="126"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0800-000011000000}" name="Next Payment Date" dataDxfId="125"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0800-000012000000}" name="Non-Call Date" dataDxfId="124"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Cusip" dataDxfId="136"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Issuer" dataDxfId="135"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Security Description" dataDxfId="134"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Issue Date" dataDxfId="133"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Maturity Date" dataDxfId="132"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Coupon" dataDxfId="131"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="Spread" dataDxfId="130"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="Current Face" dataDxfId="129" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="Factor" dataDxfId="128"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="Market Price" dataDxfId="127"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="Market Value" dataDxfId="126" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="NRSRO" dataDxfId="125"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0800-00000D000000}" name="NRSRO Rating" dataDxfId="124"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0800-00000E000000}" name="WAL" dataDxfId="123"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0800-00000F000000}" name="Par Sub" dataDxfId="122" dataCellStyle="Percent"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0800-000010000000}" name="Implied DM" dataDxfId="121"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0800-000011000000}" name="Next Payment Date" dataDxfId="120"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0800-000012000000}" name="Non-Call Date" dataDxfId="119"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -11279,8 +11279,8 @@
   <dimension ref="B1:S137"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <pane ySplit="5" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -11419,8 +11419,8 @@
       </c>
       <c r="G10" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
         <v>0</v>
       </c>
       <c r="I10" s="24" t="s">
@@ -11434,9 +11434,9 @@
       </c>
       <c r="K10" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>0.63602196422248525</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>0.63241357539312226</v>
       </c>
       <c r="M10" s="24" t="s">
         <v>19</v>
@@ -11449,9 +11449,9 @@
       </c>
       <c r="O10" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>0.46206541376586474</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>0.45944394505683056</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.2">
@@ -11474,9 +11474,9 @@
       </c>
       <c r="G11" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>8.9030464246669272E-2</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>8.8525361355995674E-2</v>
       </c>
       <c r="I11" s="24" t="s">
         <v>22</v>
@@ -11489,9 +11489,9 @@
       </c>
       <c r="K11" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>1.2717533909769945</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>1.2645382616452336</v>
       </c>
       <c r="M11" s="24" t="s">
         <v>23</v>
@@ -11504,9 +11504,9 @@
       </c>
       <c r="O11" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>0.11992969476636747</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>0.11924928906460387</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
@@ -11531,9 +11531,9 @@
       </c>
       <c r="G12" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>1.4469099818086559</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>1.4387011240818091</v>
       </c>
       <c r="I12" s="24" t="s">
         <v>25</v>
@@ -11546,9 +11546,9 @@
       </c>
       <c r="K12" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>1.2222533029628866</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>1.2153190060153674</v>
       </c>
       <c r="M12" s="24" t="s">
         <v>26</v>
@@ -11561,9 +11561,9 @@
       </c>
       <c r="O12" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>0.23094732760886286</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>0.22963707764267843</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
@@ -11588,9 +11588,9 @@
       </c>
       <c r="G13" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>9.2653029132405536</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>9.2127374085670279</v>
       </c>
       <c r="I13" s="24" t="s">
         <v>29</v>
@@ -11603,9 +11603,9 @@
       </c>
       <c r="K13" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>3.9405892175625019</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>3.9182327913482862</v>
       </c>
       <c r="M13" s="24" t="s">
         <v>30</v>
@@ -11618,9 +11618,9 @@
       </c>
       <c r="O13" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>0.31716962331811782</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>0.31537020224436069</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
@@ -11643,9 +11643,9 @@
       </c>
       <c r="G14" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>2.201563830205719</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>2.1890735409092557</v>
       </c>
       <c r="I14" s="24" t="s">
         <v>33</v>
@@ -11658,9 +11658,9 @@
       </c>
       <c r="K14" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>5.9023124411862664</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>5.8688264305164584</v>
       </c>
       <c r="M14" s="24" t="s">
         <v>34</v>
@@ -11673,9 +11673,9 @@
       </c>
       <c r="O14" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>1.1451929349207475</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>1.1386958300622934</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.2">
@@ -11700,9 +11700,9 @@
       </c>
       <c r="G15" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>0.22167532140567431</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>0.22041767497441697</v>
       </c>
       <c r="I15" s="24" t="s">
         <v>37</v>
@@ -11715,9 +11715,9 @@
       </c>
       <c r="K15" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>0.22665766076693153</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>0.22537174767397608</v>
       </c>
       <c r="M15" s="24" t="s">
         <v>38</v>
@@ -11730,9 +11730,9 @@
       </c>
       <c r="O15" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>11.037410742659349</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[coupon_Range],Table15[[#This Row],[Coupon]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>10.974791412087031</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.2">
@@ -11755,9 +11755,9 @@
       </c>
       <c r="G16" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>3.9751389493000854E-2</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>3.9525865096255296E-2</v>
       </c>
       <c r="I16" s="24" t="s">
         <v>41</v>
@@ -11770,9 +11770,9 @@
       </c>
       <c r="K16" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>0.11312775936123431</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[WAL_Range],Table14[[#This Row],[WAL]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>0.11248594356534594</v>
       </c>
       <c r="M16" s="24" t="s">
         <v>42</v>
@@ -11783,7 +11783,7 @@
       </c>
       <c r="O16" s="23">
         <f>SUBTOTAL(109,Table15[Portfolio % MV])</f>
-        <v>13.312715737039309</v>
+        <v>13.237187756157798</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
@@ -11806,9 +11806,9 @@
       </c>
       <c r="G17" s="34">
         <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
-   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>4.8481836639031058E-2</v>
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$11,
+   SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
+        <v>4.8206781173031329E-2</v>
       </c>
       <c r="I17" s="24" t="s">
         <v>42</v>
@@ -11819,7 +11819,7 @@
       </c>
       <c r="K17" s="23">
         <f>SUBTOTAL(109,Table14[Portfolio % MV])</f>
-        <v>13.312715737039301</v>
+        <v>13.237187756157791</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
@@ -11840,7 +11840,7 @@
       </c>
       <c r="G18" s="23">
         <f>SUBTOTAL(109,Table13[Portfolio % MV])</f>
-        <v>13.312715737039303</v>
+        <v>13.237187756157791</v>
       </c>
     </row>
     <row r="19" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>